<commit_message>
update rule to role.
</commit_message>
<xml_diff>
--- a/数据库设计文档v1.3.xlsx
+++ b/数据库设计文档v1.3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9815" tabRatio="971" firstSheet="5" activeTab="16"/>
+    <workbookView windowWidth="22943" windowHeight="9815" tabRatio="971" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="表目录" sheetId="1" r:id="rId1"/>
@@ -12,10 +12,10 @@
     <sheet name="BBS_Attachment_Download_User" sheetId="3" r:id="rId3"/>
     <sheet name="BBS_Category" sheetId="4" r:id="rId4"/>
     <sheet name="BBS_Global_Params" sheetId="5" r:id="rId5"/>
-    <sheet name="BBS_Rule_Group" sheetId="6" r:id="rId6"/>
-    <sheet name="BBS_Group_Right" sheetId="7" r:id="rId7"/>
+    <sheet name="BBS_Role_Group" sheetId="6" r:id="rId6"/>
+    <sheet name="BBS_Role_Group_Right" sheetId="7" r:id="rId7"/>
     <sheet name="BBS_Icon" sheetId="8" r:id="rId8"/>
-    <sheet name="BBS_Rule_Manage" sheetId="9" r:id="rId9"/>
+    <sheet name="BBS_Role_Manage" sheetId="9" r:id="rId9"/>
     <sheet name="BBS_Online" sheetId="10" r:id="rId10"/>
     <sheet name="BBS_Reply" sheetId="11" r:id="rId11"/>
     <sheet name="BBS_Special" sheetId="12" r:id="rId12"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375">
   <si>
     <t>论坛：数据库设计文档</t>
   </si>
@@ -150,13 +150,13 @@
     <t>全局参数信息</t>
   </si>
   <si>
-    <t>BBS_Rule_Group</t>
+    <t>BBS_Role_Group</t>
   </si>
   <si>
     <t>论坛权限组</t>
   </si>
   <si>
-    <t>BBS_Rule_Group_Right</t>
+    <t>BBS_Role_Group_Right</t>
   </si>
   <si>
     <t>权限组的权限表-组对应有哪些功能</t>
@@ -168,7 +168,7 @@
     <t>论坛帖子图标表</t>
   </si>
   <si>
-    <t>BBS_Rule_Manage</t>
+    <t>BBS_Role_Manage</t>
   </si>
   <si>
     <t>论坛版本权限功能表</t>
@@ -630,7 +630,7 @@
     <t>PK_BBS_Global</t>
   </si>
   <si>
-    <t>数据表名：BBS_Rule_Group</t>
+    <t>数据表名：BBS_Role_Group</t>
   </si>
   <si>
     <t>说明：论坛权限组</t>
@@ -640,6 +640,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>组</t>
     </r>
     <r>
@@ -674,7 +680,7 @@
     <t>PK_BBS_Group</t>
   </si>
   <si>
-    <t>数据表名：BBS_Group_Right</t>
+    <t>数据表名：BBS_Role_Group_Right</t>
   </si>
   <si>
     <t>说明：权限组的权限表-组对应有哪些功能</t>
@@ -684,6 +690,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>管理组</t>
     </r>
     <r>
@@ -701,6 +713,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>单个管理权限单元</t>
     </r>
     <r>
@@ -738,7 +756,7 @@
     <t>PK_BBS_Icon</t>
   </si>
   <si>
-    <t>数据表名：BBS_Rule_Manage</t>
+    <t>数据表名：BBS_Role_Manage</t>
   </si>
   <si>
     <t>说明：论坛版本权限功能表</t>
@@ -1381,6 +1399,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>所对应的版块分类</t>
     </r>
     <r>
@@ -1395,6 +1419,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>社区版块管理组</t>
     </r>
     <r>
@@ -1406,134 +1436,6 @@
       </rPr>
       <t>ID</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>用户</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color indexed="8"/>
-        <rFont val="Verdana"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ID</t>
-    </r>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>PK_BBS_UserRight</t>
-  </si>
-  <si>
-    <t>数据表名：BBS_Vote</t>
-  </si>
-  <si>
-    <t>说明：论坛投票帖子</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>tinyint</t>
-  </si>
-  <si>
-    <t>类别:如0:单行1:多选</t>
-  </si>
-  <si>
-    <t>投票总数</t>
-  </si>
-  <si>
-    <t>user_count</t>
-  </si>
-  <si>
-    <t>投票用户总数</t>
-  </si>
-  <si>
-    <t>limit</t>
-  </si>
-  <si>
-    <t>权限限制[分值限制,默认0分不限制]</t>
-  </si>
-  <si>
-    <t>available_day</t>
-  </si>
-  <si>
-    <t>投票有效天数[0默认不限制]</t>
-  </si>
-  <si>
-    <t>look_mode</t>
-  </si>
-  <si>
-    <t>查看方式[0:直接查看;1:投票后查看]</t>
-  </si>
-  <si>
-    <t>投票创建时间</t>
-  </si>
-  <si>
-    <t>PK_ForumVote</t>
-  </si>
-  <si>
-    <t>数据表名：BBS_Vote_Item</t>
-  </si>
-  <si>
-    <t>说明：论坛投标帖的投票项</t>
-  </si>
-  <si>
-    <t>vote_id</t>
-  </si>
-  <si>
-    <t>投票ID</t>
-  </si>
-  <si>
-    <t>投票项目名称</t>
-  </si>
-  <si>
-    <t>投票数</t>
-  </si>
-  <si>
-    <t>投票项目创建时间</t>
-  </si>
-  <si>
-    <t>PK_BBS_VoteItem</t>
-  </si>
-  <si>
-    <t>数据表名：BBS_Vote_User</t>
-  </si>
-  <si>
-    <t>说明：论坛投票帖的投票用户</t>
-  </si>
-  <si>
-    <t>vote_item_id</t>
-  </si>
-  <si>
-    <t>投票项目ID</t>
-  </si>
-  <si>
-    <t>投票时间</t>
-  </si>
-  <si>
-    <t>PK_BBS_VoteUser</t>
-  </si>
-  <si>
-    <t>数据表名：Error_Logs</t>
-  </si>
-  <si>
-    <t>说明：数据库执行错误日志</t>
-  </si>
-  <si>
-    <t>page_url</t>
-  </si>
-  <si>
-    <t>错误页面</t>
-  </si>
-  <si>
-    <t>error_message</t>
-  </si>
-  <si>
-    <t>错误信息</t>
   </si>
   <si>
     <r>
@@ -1556,6 +1458,120 @@
     </r>
   </si>
   <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>PK_BBS_UserRight</t>
+  </si>
+  <si>
+    <t>数据表名：BBS_Vote</t>
+  </si>
+  <si>
+    <t>说明：论坛投票帖子</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>tinyint</t>
+  </si>
+  <si>
+    <t>类别:如0:单行1:多选</t>
+  </si>
+  <si>
+    <t>投票总数</t>
+  </si>
+  <si>
+    <t>user_count</t>
+  </si>
+  <si>
+    <t>投票用户总数</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>权限限制[分值限制,默认0分不限制]</t>
+  </si>
+  <si>
+    <t>available_day</t>
+  </si>
+  <si>
+    <t>投票有效天数[0默认不限制]</t>
+  </si>
+  <si>
+    <t>look_mode</t>
+  </si>
+  <si>
+    <t>查看方式[0:直接查看;1:投票后查看]</t>
+  </si>
+  <si>
+    <t>投票创建时间</t>
+  </si>
+  <si>
+    <t>PK_ForumVote</t>
+  </si>
+  <si>
+    <t>数据表名：BBS_Vote_Item</t>
+  </si>
+  <si>
+    <t>说明：论坛投标帖的投票项</t>
+  </si>
+  <si>
+    <t>vote_id</t>
+  </si>
+  <si>
+    <t>投票ID</t>
+  </si>
+  <si>
+    <t>投票项目名称</t>
+  </si>
+  <si>
+    <t>投票数</t>
+  </si>
+  <si>
+    <t>投票项目创建时间</t>
+  </si>
+  <si>
+    <t>PK_BBS_VoteItem</t>
+  </si>
+  <si>
+    <t>数据表名：BBS_Vote_User</t>
+  </si>
+  <si>
+    <t>说明：论坛投票帖的投票用户</t>
+  </si>
+  <si>
+    <t>vote_item_id</t>
+  </si>
+  <si>
+    <t>投票项目ID</t>
+  </si>
+  <si>
+    <t>投票时间</t>
+  </si>
+  <si>
+    <t>PK_BBS_VoteUser</t>
+  </si>
+  <si>
+    <t>数据表名：Error_Logs</t>
+  </si>
+  <si>
+    <t>说明：数据库执行错误日志</t>
+  </si>
+  <si>
+    <t>page_url</t>
+  </si>
+  <si>
+    <t>错误页面</t>
+  </si>
+  <si>
+    <t>error_message</t>
+  </si>
+  <si>
+    <t>错误信息</t>
+  </si>
+  <si>
     <t>PK_ErrorLogs</t>
   </si>
   <si>
@@ -1673,10 +1689,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="[DBNum1][$-804]General"/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="11">
@@ -2283,8 +2299,8 @@
   <sheetPr/>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -2644,10 +2660,10 @@
     <hyperlink ref="B9" location="BBS_Attachment_Download_User!A1" display="BBS_Attachment_Download_User"/>
     <hyperlink ref="B10" location="BBS_Category!A1" display="BBS_Category"/>
     <hyperlink ref="B11" location="BBS_Global_Params!A1" display="BBS_Global_Params"/>
-    <hyperlink ref="B12" location="BBS_Rule_Group!A1" display="BBS_Rule_Group"/>
-    <hyperlink ref="B13" location="BBS_Group_Right!A1" display="BBS_Rule_Group_Right"/>
+    <hyperlink ref="B12" location="BBS_Role_Group!A1" display="BBS_Role_Group"/>
+    <hyperlink ref="B13" location="BBS_Role_Group_Right!A1" display="BBS_Role_Group_Right"/>
     <hyperlink ref="B14" location="BBS_Icon!A1" display="BBS_Icon"/>
-    <hyperlink ref="B15" location="BBS_Rule_Manage!A1" display="BBS_Rule_Manage"/>
+    <hyperlink ref="B15" location="BBS_Role_Manage!A1" display="BBS_Role_Manage"/>
     <hyperlink ref="B16" location="BBS_Online!A1" display="BBS_Online"/>
     <hyperlink ref="B17" location="BBS_Reply!A1" display="BBS_Reply"/>
     <hyperlink ref="B18" location="BBS_Special!A1" display="BBS_Special"/>
@@ -4755,7 +4771,7 @@
   <sheetPr/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -4788,7 +4804,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" ht="15.15" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -4805,7 +4821,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" ht="15.15" spans="1:5">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -4822,7 +4838,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" ht="15.15" spans="1:5">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -4839,7 +4855,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" ht="15.15" spans="1:5">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -4856,7 +4872,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" ht="15.15" spans="1:5">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -4873,7 +4889,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" ht="15.15" spans="1:5">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -4890,7 +4906,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" ht="15.15" spans="1:5">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -5991,7 +6007,7 @@
         <v>75</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>349</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" ht="35.55" spans="1:1">
@@ -6018,7 +6034,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>103</v>
@@ -6055,7 +6071,7 @@
   <sheetData>
     <row r="1" ht="24" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -6064,7 +6080,7 @@
     </row>
     <row r="2" ht="21.75" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -6107,7 +6123,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" ht="15.15" spans="1:5">
@@ -6115,7 +6131,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>97</v>
@@ -6132,7 +6148,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>84</v>
@@ -6141,7 +6157,7 @@
         <v>75</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" ht="15.15" spans="1:5">
@@ -6149,7 +6165,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>71</v>
@@ -6158,7 +6174,7 @@
         <v>75</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>349</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" ht="15.15" spans="1:5">
@@ -6166,7 +6182,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>71</v>
@@ -6175,7 +6191,7 @@
         <v>75</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" ht="35.55" spans="1:1">
@@ -6202,7 +6218,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>103</v>
@@ -6239,7 +6255,7 @@
   <sheetData>
     <row r="1" ht="24" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -6248,7 +6264,7 @@
     </row>
     <row r="2" ht="21.75" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -6291,7 +6307,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" ht="15.15" spans="1:5">
@@ -6299,7 +6315,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>97</v>
@@ -6308,7 +6324,7 @@
         <v>75</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" ht="15.15" spans="1:5">
@@ -6325,7 +6341,7 @@
         <v>75</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" ht="15.15" spans="1:5">
@@ -6342,7 +6358,7 @@
         <v>75</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" ht="15.15" spans="1:5">
@@ -6350,7 +6366,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>84</v>
@@ -6359,7 +6375,7 @@
         <v>75</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" ht="35.55" spans="1:1">
@@ -6386,7 +6402,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>103</v>
@@ -6439,7 +6455,7 @@
   <sheetData>
     <row r="1" ht="24" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -6448,7 +6464,7 @@
     </row>
     <row r="2" ht="21.75" customHeight="1" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -6491,7 +6507,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" ht="15.15" spans="1:5">
@@ -6508,7 +6524,7 @@
         <v>75</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="7" ht="15.15" spans="1:5">
@@ -6516,7 +6532,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>84</v>
@@ -6525,7 +6541,7 @@
         <v>75</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" ht="35.55" spans="1:1">
@@ -6552,7 +6568,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>103</v>
@@ -7388,7 +7404,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -7439,7 +7455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" ht="15.15" spans="1:5">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -7456,7 +7472,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" ht="15.15" spans="1:5">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -7473,7 +7489,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" ht="15.15" spans="1:5">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -7490,7 +7506,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" ht="15.15" spans="1:5">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -7556,7 +7572,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -7605,7 +7621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" ht="15.15" spans="1:5">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -7622,7 +7638,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" ht="15.15" spans="1:5">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -7656,7 +7672,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" ht="15.15" spans="1:5">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -7905,8 +7921,8 @@
   <sheetPr/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -7956,7 +7972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" ht="15.15" spans="1:5">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -7973,7 +7989,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" ht="15.15" spans="1:5">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -8007,7 +8023,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" ht="15.15" spans="1:5">
       <c r="A8" s="5">
         <v>4</v>
       </c>

</xml_diff>